<commit_message>
Ugggh digikey made me add their part numbers. Hrmph.
</commit_message>
<xml_diff>
--- a/oresat-proto-card-bom.xlsx
+++ b/oresat-proto-card-bom.xlsx
@@ -19,19 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="62" count="62">
-  <si>
-    <t>Cnt</t>
-  </si>
-  <si>
-    <t>P/DNP</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>C11, C16</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12" count="12">
   <si>
     <t>P</t>
   </si>
@@ -39,22 +27,10 @@
     <t>Samsung</t>
   </si>
   <si>
-    <t>CL05C200JB51PNC</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
-    <t>C12</t>
-  </si>
-  <si>
-    <t>C1, C3, C9, C17, C22</t>
-  </si>
-  <si>
-    <t>CL05B104KO5NNNC</t>
-  </si>
-  <si>
-    <t>C2</t>
+    <t>Digi-Key</t>
   </si>
   <si>
     <t>NP</t>
@@ -63,145 +39,19 @@
     <t>-</t>
   </si>
   <si>
-    <t>C4, C5, C10</t>
-  </si>
-  <si>
-    <t>C7</t>
-  </si>
-  <si>
-    <t>CM1, CM2, CM3</t>
-  </si>
-  <si>
-    <t>Molex</t>
-  </si>
-  <si>
-    <t>73300-0020</t>
-  </si>
-  <si>
-    <t>D1, D2</t>
-  </si>
-  <si>
-    <t>J1</t>
-  </si>
-  <si>
     <t>Samtec</t>
-  </si>
-  <si>
-    <t>TFM-110-01-L-D-RA</t>
   </si>
   <si>
     <t>N</t>
   </si>
   <si>
-    <t>J2, J3, J4</t>
-  </si>
-  <si>
-    <t>J6</t>
-  </si>
-  <si>
-    <t>TFM-120-01-L-D-RA</t>
-  </si>
-  <si>
-    <t>J7</t>
-  </si>
-  <si>
-    <t>L2</t>
-  </si>
-  <si>
-    <t>ECS</t>
-  </si>
-  <si>
-    <t>ECS-MPI4040R4-6R8-R</t>
-  </si>
-  <si>
-    <t>Q3, Q4</t>
-  </si>
-  <si>
-    <t>Diodes Inc</t>
-  </si>
-  <si>
-    <t>DMP3050LVT-7</t>
-  </si>
-  <si>
-    <t>Q5, Q6</t>
-  </si>
-  <si>
-    <t>R1, R2, R3, R12</t>
-  </si>
-  <si>
     <t>RC1005F6653CS</t>
   </si>
   <si>
-    <t>R29</t>
-  </si>
-  <si>
-    <t>R31, R33</t>
-  </si>
-  <si>
-    <t>R4, R24, R25</t>
-  </si>
-  <si>
-    <t>R5, R6, R8, R9, R10, R11, R13, R14, R19, R20, R21, R22, R23, R32, R34, R36, R37</t>
-  </si>
-  <si>
-    <t>R7, R17, R26, R27, R28, R30, R35, R38</t>
-  </si>
-  <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>Texas Instruments</t>
-  </si>
-  <si>
-    <t>TCAN330GDCNT</t>
-  </si>
-  <si>
-    <t>U3</t>
+    <t>1276-4275-1-ND</t>
   </si>
   <si>
     <t>Maxim</t>
-  </si>
-  <si>
-    <t>MAX7310ATE</t>
-  </si>
-  <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>MAX4211CETE</t>
-  </si>
-  <si>
-    <t>U5</t>
-  </si>
-  <si>
-    <t>TI</t>
-  </si>
-  <si>
-    <t>TPS62111RSA</t>
-  </si>
-  <si>
-    <t>U6</t>
-  </si>
-  <si>
-    <t>STMicroelectronics</t>
-  </si>
-  <si>
-    <t>U7</t>
-  </si>
-  <si>
-    <t>Microchip</t>
-  </si>
-  <si>
-    <t>MCP1703AT-3302E/CB</t>
-  </si>
-  <si>
-    <t>X1</t>
-  </si>
-  <si>
-    <t>ECS Inc.</t>
-  </si>
-  <si>
-    <t>ECS-160-10-36Q-ES-TR</t>
   </si>
   <si>
     <t>??</t>
@@ -293,7 +143,7 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -305,8 +155,9 @@
     <col min="5" max="5" style="0" width="26.426983173076927" customWidth="1"/>
     <col min="6" max="6" style="0" width="57.567968750000006" customWidth="1"/>
     <col min="7" max="7" style="1" width="9.142307692307693"/>
-    <col min="8" max="8" style="0" width="42.71171875" customWidth="1"/>
-    <col min="9" max="12" style="0" width="9.142307692307693"/>
+    <col min="8" max="8" style="0" width="8.999459134615385" customWidth="1"/>
+    <col min="9" max="9" style="0" width="27.56977163461539" customWidth="1"/>
+    <col min="10" max="12" style="0" width="9.142307692307693"/>
     <col min="13" max="13" style="0" width="27.855468750000004" customWidth="1"/>
     <col min="14" max="14" style="0" width="29.712500000000002" customWidth="1"/>
     <col min="15" max="15" style="0" width="9.142307692307693"/>
@@ -411,16 +262,20 @@
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:16" ht="13.5">
-      <c r="A7" s="2" t="s">
-        <v>0</v>
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Cnt</t>
+        </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
           <t>Part References</t>
         </is>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>1</v>
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>P/DNP</t>
+        </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
@@ -442,25 +297,36 @@
           <t>Generic</t>
         </is>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>2</v>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>Dist</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>Dist Part Number</t>
+        </is>
       </c>
     </row>
     <row r="8" spans="1:16" ht="13.5">
       <c r="A8">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
-        <v>3</v>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>C11, C16</t>
+        </is>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E8" t="s">
-        <v>6</v>
+        <v>1</v>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>CL05C200JB51PNC</t>
+        </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -468,21 +334,31 @@
         </is>
       </c>
       <c r="G8" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>1276-6601-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="9" spans="1:16" ht="13.5">
       <c r="A9">
         <v>1</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>C12</t>
+        </is>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D9" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
@@ -495,24 +371,36 @@
         </is>
       </c>
       <c r="G9" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>3</v>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>1276-3031-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="10" spans="1:16" ht="13.5">
       <c r="A10">
         <v>5</v>
       </c>
-      <c r="B10" t="s">
-        <v>9</v>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>C1, C3, C9, C17, C22</t>
+        </is>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" t="s">
-        <v>10</v>
+        <v>1</v>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>CL05B104KO5NNNC</t>
+        </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -520,24 +408,34 @@
         </is>
       </c>
       <c r="G10" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>1276-1001-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="11" spans="1:16" ht="13.5">
       <c r="A11">
         <v>1</v>
       </c>
-      <c r="B11" t="s">
-        <v>11</v>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>C2</t>
+        </is>
       </c>
       <c r="C11" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -545,21 +443,29 @@
         </is>
       </c>
       <c r="G11" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="13.5">
       <c r="A12">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
-        <v>14</v>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>C4, C5, C10</t>
+        </is>
       </c>
       <c r="C12" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
@@ -572,18 +478,28 @@
         </is>
       </c>
       <c r="G12" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>1276-1184-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="13" spans="1:16" ht="13.5">
-      <c r="B13" t="s">
-        <v>15</v>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>C7</t>
+        </is>
       </c>
       <c r="C13" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
@@ -596,24 +512,38 @@
         </is>
       </c>
       <c r="G13" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>1276-2872-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="14" spans="1:16" ht="13.5">
       <c r="A14">
         <v>3</v>
       </c>
-      <c r="B14" t="s">
-        <v>16</v>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>CM1, CM2, CM3</t>
+        </is>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" t="s">
-        <v>18</v>
+        <v>0</v>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Molex</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>73300-0020</t>
+        </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -621,18 +551,28 @@
         </is>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>WM10772-ND</t>
+        </is>
       </c>
     </row>
     <row r="15" spans="1:16" ht="13.5">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" t="s">
-        <v>19</v>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>D1, D2</t>
+        </is>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
@@ -650,7 +590,15 @@
         </is>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>3</v>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>754-2193-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="16" spans="1:16" ht="13.5">
@@ -663,7 +611,7 @@
         </is>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -681,24 +629,36 @@
         </is>
       </c>
       <c r="G16" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H16" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>1830-1071-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="17" spans="1:16" ht="13.5">
       <c r="A17">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
-        <v>20</v>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>J1</t>
+        </is>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s">
-        <v>22</v>
+        <v>6</v>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>TFM-110-01-L-D-RA</t>
+        </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -706,18 +666,28 @@
         </is>
       </c>
       <c r="G17" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>SAM10113-ND</t>
+        </is>
       </c>
     </row>
     <row r="18" spans="1:16" ht="13.5">
       <c r="A18">
         <v>3</v>
       </c>
-      <c r="B18" t="s">
-        <v>24</v>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>J2, J3, J4</t>
+        </is>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
@@ -735,24 +705,36 @@
         </is>
       </c>
       <c r="G18" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>3</v>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>A118077CT-ND</t>
+        </is>
       </c>
     </row>
     <row r="19" spans="1:16" ht="13.5">
       <c r="A19">
         <v>1</v>
       </c>
-      <c r="B19" t="s">
-        <v>25</v>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>J6</t>
+        </is>
       </c>
       <c r="C19" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
-        <v>26</v>
+        <v>6</v>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>TFM-120-01-L-D-RA</t>
+        </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -760,21 +742,31 @@
         </is>
       </c>
       <c r="G19" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>3</v>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>SAM10145-ND</t>
+        </is>
       </c>
     </row>
     <row r="20" spans="1:16" ht="13.5">
       <c r="A20">
         <v>1</v>
       </c>
-      <c r="B20" t="s">
-        <v>27</v>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>J7</t>
+        </is>
       </c>
       <c r="C20" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -787,7 +779,15 @@
         </is>
       </c>
       <c r="G20" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H20" t="s">
+        <v>3</v>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>SAM13160CT-ND</t>
+        </is>
       </c>
     </row>
     <row r="21" spans="1:16" ht="13.5">
@@ -800,13 +800,13 @@
         </is>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -814,24 +814,36 @@
         </is>
       </c>
       <c r="G21" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H21" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="13.5">
       <c r="A22">
         <v>1</v>
       </c>
-      <c r="B22" t="s">
-        <v>28</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
       </c>
       <c r="C22" t="s">
-        <v>4</v>
-      </c>
-      <c r="D22" t="s">
-        <v>29</v>
-      </c>
-      <c r="E22" t="s">
-        <v>30</v>
+        <v>0</v>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>ECS</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>ECS-MPI4040R4-6R8-R</t>
+        </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -839,24 +851,38 @@
         </is>
       </c>
       <c r="G22" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
+        <v>3</v>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>XC2337CT-ND</t>
+        </is>
       </c>
     </row>
     <row r="23" spans="1:16" ht="13.5">
       <c r="A23">
         <v>2</v>
       </c>
-      <c r="B23" t="s">
-        <v>31</v>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Q3, Q4</t>
+        </is>
       </c>
       <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" t="s">
-        <v>33</v>
+        <v>0</v>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Diodes Inc</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>DMP3050LVT-7</t>
+        </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -864,18 +890,28 @@
         </is>
       </c>
       <c r="G23" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H23" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>DMP3050LVT-7DICT-ND	</t>
+        </is>
       </c>
     </row>
     <row r="24" spans="1:16" ht="13.5">
       <c r="A24">
         <v>2</v>
       </c>
-      <c r="B24" t="s">
-        <v>34</v>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Q5, Q6</t>
+        </is>
       </c>
       <c r="C24" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -893,24 +929,34 @@
         </is>
       </c>
       <c r="G24" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>3</v>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>1727-2307-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="25" spans="1:16" ht="13.5">
       <c r="A25">
         <v>4</v>
       </c>
-      <c r="B25" t="s">
-        <v>35</v>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>R1, R2, R3, R12</t>
+        </is>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -918,21 +964,29 @@
         </is>
       </c>
       <c r="G25" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H25" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="13.5">
       <c r="A26">
         <v>1</v>
       </c>
-      <c r="B26" t="s">
-        <v>37</v>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>R29</t>
+        </is>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D26" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
@@ -945,24 +999,34 @@
         </is>
       </c>
       <c r="G26" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H26" t="s">
+        <v>3</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>1276-6173-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="27" spans="1:16" ht="13.5">
       <c r="A27">
         <v>2</v>
       </c>
-      <c r="B27" t="s">
-        <v>38</v>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>R31, R33</t>
+        </is>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D27" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -970,21 +1034,29 @@
         </is>
       </c>
       <c r="G27" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H27" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="13.5">
       <c r="A28">
         <v>3</v>
       </c>
-      <c r="B28" t="s">
-        <v>39</v>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>R4, R24, R25</t>
+        </is>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D28" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
@@ -997,24 +1069,34 @@
         </is>
       </c>
       <c r="G28" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H28" t="s">
+        <v>3</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>1276-3429-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="29" spans="1:16" ht="13.5">
       <c r="A29">
         <v>17</v>
       </c>
-      <c r="B29" t="s">
-        <v>40</v>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>R5, R6, R8, R9, R10, R11, R13, R14, R19, R20, R21, R22, R23, R32, R34, R36, R37</t>
+        </is>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -1022,21 +1104,29 @@
         </is>
       </c>
       <c r="G29" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H29" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="13.5">
       <c r="A30">
         <v>8</v>
       </c>
-      <c r="B30" t="s">
-        <v>41</v>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>R7, R17, R26, R27, R28, R30, R35, R38</t>
+        </is>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D30" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -1049,24 +1139,38 @@
         </is>
       </c>
       <c r="G30" t="s">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="H30" t="s">
+        <v>3</v>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>1276-3431-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="31" spans="1:16" ht="13.5">
       <c r="A31">
         <v>1</v>
       </c>
-      <c r="B31" t="s">
-        <v>42</v>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>U2</t>
+        </is>
       </c>
       <c r="C31" t="s">
-        <v>4</v>
-      </c>
-      <c r="D31" t="s">
-        <v>43</v>
-      </c>
-      <c r="E31" t="s">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Texas Instruments</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>TCAN330GDCNT</t>
+        </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -1074,24 +1178,36 @@
         </is>
       </c>
       <c r="G31" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H31" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>296-44211-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="32" spans="1:16" ht="13.5">
       <c r="A32">
         <v>1</v>
       </c>
-      <c r="B32" t="s">
-        <v>45</v>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>U3</t>
+        </is>
       </c>
       <c r="C32" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D32" t="s">
-        <v>46</v>
-      </c>
-      <c r="E32" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>MAX7310ATE</t>
+        </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -1099,24 +1215,36 @@
         </is>
       </c>
       <c r="G32" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H32" t="s">
+        <v>3</v>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>MAX7310ATE+-ND</t>
+        </is>
       </c>
     </row>
     <row r="33" spans="1:16" ht="13.5">
       <c r="A33">
         <v>1</v>
       </c>
-      <c r="B33" t="s">
-        <v>48</v>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>U4</t>
+        </is>
       </c>
       <c r="C33" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D33" t="s">
-        <v>46</v>
-      </c>
-      <c r="E33" t="s">
-        <v>49</v>
+        <v>10</v>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>MAX4211CETE</t>
+        </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -1124,24 +1252,38 @@
         </is>
       </c>
       <c r="G33" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H33" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>MAX4211CETE+-ND</t>
+        </is>
       </c>
     </row>
     <row r="34" spans="1:16" ht="13.5">
       <c r="A34">
         <v>1</v>
       </c>
-      <c r="B34" t="s">
-        <v>50</v>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>U5</t>
+        </is>
       </c>
       <c r="C34" t="s">
-        <v>4</v>
-      </c>
-      <c r="D34" t="s">
-        <v>51</v>
-      </c>
-      <c r="E34" t="s">
-        <v>52</v>
+        <v>0</v>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>TI</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>TPS62111RSA</t>
+        </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -1149,21 +1291,33 @@
         </is>
       </c>
       <c r="G34" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H34" t="s">
+        <v>3</v>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>296-37681-1-ND</t>
+        </is>
       </c>
     </row>
     <row r="35" spans="1:16" ht="13.5">
       <c r="A35">
         <v>1</v>
       </c>
-      <c r="B35" t="s">
-        <v>53</v>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>U6</t>
+        </is>
       </c>
       <c r="C35" t="s">
-        <v>4</v>
-      </c>
-      <c r="D35" t="s">
-        <v>54</v>
+        <v>0</v>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>STMicroelectronics</t>
+        </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
@@ -1176,24 +1330,38 @@
         </is>
       </c>
       <c r="G35" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H35" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>497-14647-ND</t>
+        </is>
       </c>
     </row>
     <row r="36" spans="1:16" ht="13.5">
       <c r="A36">
         <v>1</v>
       </c>
-      <c r="B36" t="s">
-        <v>55</v>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>U7</t>
+        </is>
       </c>
       <c r="C36" t="s">
-        <v>4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>56</v>
-      </c>
-      <c r="E36" t="s">
-        <v>57</v>
+        <v>0</v>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Microchip</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>MCP1703AT-3302E/CB</t>
+        </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -1201,24 +1369,38 @@
         </is>
       </c>
       <c r="G36" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H36" t="s">
+        <v>3</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>MCP1703AT-3302E/CBCT-ND</t>
+        </is>
       </c>
     </row>
     <row r="37" spans="1:16" ht="13.5">
       <c r="A37">
         <v>1</v>
       </c>
-      <c r="B37" t="s">
-        <v>58</v>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>X1</t>
+        </is>
       </c>
       <c r="C37" t="s">
-        <v>4</v>
-      </c>
-      <c r="D37" t="s">
-        <v>59</v>
-      </c>
-      <c r="E37" t="s">
-        <v>60</v>
+        <v>0</v>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>ECS Inc.</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>ECS-160-10-36Q-ES-TR</t>
+        </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -1226,7 +1408,15 @@
         </is>
       </c>
       <c r="G37" t="s">
-        <v>23</v>
+        <v>7</v>
+      </c>
+      <c r="H37" t="s">
+        <v>3</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>XC2181CT-ND</t>
+        </is>
       </c>
     </row>
     <row r="39" spans="1:16" ht="13.5">
@@ -1247,8 +1437,10 @@
           <t>Date</t>
         </is>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>2</v>
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
       </c>
     </row>
     <row r="42" spans="1:16" ht="13.5">
@@ -1273,7 +1465,7 @@
         </is>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C43" s="0" t="inlineStr">
         <is>
@@ -1288,7 +1480,7 @@
         </is>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="C44" s="0" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
fixed an error where Pout was not routed to an ADC pin
</commit_message>
<xml_diff>
--- a/oresat-proto-card-bom.xlsx
+++ b/oresat-proto-card-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="179">
   <si>
     <t xml:space="preserve">Bill Of Materials for OreSat Prototype Card</t>
   </si>
@@ -28,10 +28,10 @@
     <t xml:space="preserve">source file: oresat-proto-card.sch</t>
   </si>
   <si>
-    <t xml:space="preserve">Last modified: 2019/12/06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PCB version: 3.3</t>
+    <t xml:space="preserve">Last modified: 2020/01/07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PCB version: 4.0</t>
   </si>
   <si>
     <t xml:space="preserve">P/DNP = </t>
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Dist Part Number</t>
   </si>
   <si>
-    <t xml:space="preserve">R31, R33</t>
+    <t xml:space="preserve">R66, R68</t>
   </si>
   <si>
     <t xml:space="preserve">P</t>
@@ -85,10 +85,7 @@
     <t xml:space="preserve">Yageo</t>
   </si>
   <si>
-    <t xml:space="preserve">RC0402JR-070RL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 0 Ohms, 1/16W, 0402</t>
+    <t xml:space="preserve">RC0603JR-070RL</t>
   </si>
   <si>
     <t xml:space="preserve">Y</t>
@@ -97,22 +94,29 @@
     <t xml:space="preserve">Digi-Key</t>
   </si>
   <si>
-    <t xml:space="preserve">311-0.0JRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R4, R25, R41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-07100RL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 100 Ohms ±1%, 1/16W, 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-100LRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R29</t>
+    <t xml:space="preserve">311-0.0GRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-0710RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-10.0HRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R60, R80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-07100RL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-100HRCT-ND
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R64</t>
   </si>
   <si>
     <t xml:space="preserve">Stackpole</t>
@@ -121,13 +125,13 @@
     <t xml:space="preserve">CSR1206FTR100</t>
   </si>
   <si>
-    <t xml:space="preserve">Resistor, 100 mOhms ±1% 1/2W Chip Resistor 1206</t>
+    <t xml:space="preserve">100m</t>
   </si>
   <si>
     <t xml:space="preserve">CSR1206FTR100CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">C1, C3, C9, C17, C22</t>
+    <t xml:space="preserve">C3, C13, C14, C19, C20, C21</t>
   </si>
   <si>
     <t xml:space="preserve">Samsung</t>
@@ -136,37 +140,37 @@
     <t xml:space="preserve">CL05B104KO5NNNC</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacitor, 0.1µF, ±10%, 16V,  X7R, 0402</t>
+    <t xml:space="preserve">100n</t>
   </si>
   <si>
     <t xml:space="preserve">1276-1001-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">R7, R15, R17, R26, R27, R28, R30, R35, R38, R42, R24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-0710KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 10 kOhms ±1%, 1/16W, 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-10.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C7</t>
+    <t xml:space="preserve">R61, R62, R63, R65, R70, R73, R77, R81, R47, R49, R74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNCP0603FTD10K0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RNCP0603FTD10K0CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C9</t>
   </si>
   <si>
     <t xml:space="preserve">CL21B106KOQNNNG</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacitor,10µF, ±10%, 16V, X7R, 0805</t>
+    <t xml:space="preserve">10u</t>
   </si>
   <si>
     <t xml:space="preserve">1276-6472-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">X1</t>
+    <t xml:space="preserve">X2</t>
   </si>
   <si>
     <t xml:space="preserve">ECS Inc.</t>
@@ -175,124 +179,112 @@
     <t xml:space="preserve">ECS-160-10-36Q-ES-TR</t>
   </si>
   <si>
-    <t xml:space="preserve">16MHz ±30ppm Crystal 10pF </t>
+    <t xml:space="preserve">16MHZ-2.5x2mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">XC2181CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R79, R83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RC0603FR-071ML</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1.00MHRCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C11, C17, C22, C23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC0603KRX5R7BB105</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-1444-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R3, R17, R48, R50, R51, R76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERA-3AEB272V</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.7k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P2.7KDBCT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C15, C18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CL05C200JB51PNC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-6601-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Murata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GRM21BD71A226ME44L</t>
+  </si>
+  <si>
+    <t xml:space="preserve">22u</t>
+  </si>
+  <si>
+    <t xml:space="preserve">490-9959-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R78, R82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TE Connectivity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CRGCQ0603F330K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">330k</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A129718CT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ECS-MPI4040R4-6R8-R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6.8u</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
   </si>
   <si>
-    <t xml:space="preserve">XC2181CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R18, R44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-071ML</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 1 MOhms ±1%, 1/16W, 0402 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-1.00MLRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C4, C5, C6, C10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CC0603KRX7R7BB105</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor, 1µF, ±10%, 16V, X7R, 0603 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-1446-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R1, R2, R3, R12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TE Connectivity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CRGCQ0402F2K7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 2.7 kOhms ±1%, 1/16W </t>
-  </si>
-  <si>
-    <t xml:space="preserve">A129632CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C11, C16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CL05C200JB51PNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor, 20pF ±5% 50V, NP0, 0402 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-6601-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Murata</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GRM21BD71A226ME44L</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Capacitor, 22µF ±20%, 10V, X7T 0805</t>
-  </si>
-  <si>
-    <t xml:space="preserve">490-9959-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R16, R43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vishay</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MCS04020C3303FE000</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 330 kOhms ±1%, 1/10W, 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">749-1575-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R39, R40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC0402FR-0747KL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 47 kOhms ±1%, 1/16W, 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">311-47.0KLRCT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ECS-MPI4040R4-6R8-R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Inductor, 6.8µH, 2.4A, 91mOhm, Nonstandard</t>
-  </si>
-  <si>
     <t xml:space="preserve">XC2337CT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">D3, D4</t>
+    <t xml:space="preserve">D5, D7</t>
   </si>
   <si>
     <t xml:space="preserve">Inolux</t>
@@ -301,13 +293,13 @@
     <t xml:space="preserve">IN-S63AT5A</t>
   </si>
   <si>
-    <t xml:space="preserve">LED, Amber, 0603  </t>
+    <t xml:space="preserve">AMBER</t>
   </si>
   <si>
     <t xml:space="preserve">1830-1064-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Q1</t>
+    <t xml:space="preserve">Q10</t>
   </si>
   <si>
     <t xml:space="preserve">Diodes Inc</t>
@@ -316,163 +308,133 @@
     <t xml:space="preserve">DMP2240UDM</t>
   </si>
   <si>
-    <t xml:space="preserve">Mosfet Array 2 P-Channel, 20V, 2A, SOT-26 </t>
-  </si>
-  <si>
     <t xml:space="preserve">DMP2240UDMDICT-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">J5</t>
+    <t xml:space="preserve">D3, D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rohm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SML-E12M8WT86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GREEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">511-1584-1-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CM1, CM2, CM3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Molex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73300-0020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J-MOLEX-SMPM-73300-003X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">WM10772-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samtec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFM-110-01-L-D-RA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">J-SAMTEC-TFM-110-X1-XXX-D-RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Digikey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAM10113-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TFM-120-01-L-D-RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J-SAMTEC-TFM-120-X1-XXX-D-RA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAM10145-ND </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Maxim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX4211FETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX4211FETE+-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX7310ATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MAX7310ATE+-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">U11, U12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microchip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIC842LYC5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q2, Q7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMP3050LVT-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOSFET-PCH-SOT23-6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DMP3050LVT-7DICT-ND</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C8</t>
   </si>
   <si>
     <t xml:space="preserve">NP</t>
   </si>
   <si>
-    <t xml:space="preserve">-</t>
+    <t xml:space="preserve">R39, R40, R45, R46, R52, R53, R54, R55, R56, R57, R58, R59, R67, R69, R71, R72, R75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1276-4275-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">J7</t>
   </si>
   <si>
-    <t xml:space="preserve">Samtec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FTSH-105-01-F-DV-K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector Header Surface Mount 10 position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAM13160CT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1, D2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rohm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SML-E12M8WT86</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LED, Green, 0603 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">511-1584-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CM1, CM2, CM3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Molex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">73300-0020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector Plug, Male Pin, 50Ohm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">WM10772-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TFM-110-01-L-D-RA </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector Header Through Hole, Right Angle, 20 position</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Digikey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAM10113-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TFM-120-01-L-D-RA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Connector Header Through Hole, Right Angle, 40 position  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAM10145-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Maxim</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX4211FETE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Current Monitor Regulator, High-Side, 16-TQFN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX4211FETE+-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX7310ATE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I/O Expander, I²C, 16-TQFN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAX7310ATE+-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U1, U7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Microchip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIC842LYC5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Comparator with Voltage Reference, Push-Pull, SC-70-5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">576-2927-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q3, Q4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMP3050LVT-7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P-Channel, 30V 4.5A, TSOT-26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DMP3050LVT-7DICT-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R5, R6, R8, R9, R10, R11, R13, R14, R19, R20, R21, R22, R23, R32, R34, R36, R37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RC1005F6653CS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Resistor, 665 kOhms ±1%, 1/16W, 0402</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1276-4275-1-ND</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q5, Q6</t>
+    <t xml:space="preserve">Wurth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ORESAT-DEBUG-CONNECTOR-SOLAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q8, Q9</t>
   </si>
   <si>
     <t xml:space="preserve">Nexperia</t>
@@ -481,13 +443,13 @@
     <t xml:space="preserve">PMV45EN2R</t>
   </si>
   <si>
-    <t xml:space="preserve">N-Channel, 30V 4.1A, TO-236AB</t>
+    <t xml:space="preserve">PMV45EN</t>
   </si>
   <si>
     <t xml:space="preserve">1727-2307-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">U6</t>
+    <t xml:space="preserve">U7</t>
   </si>
   <si>
     <t xml:space="preserve">STMicroelectronics</t>
@@ -496,13 +458,13 @@
     <t xml:space="preserve">STM32F042K6T7</t>
   </si>
   <si>
-    <t xml:space="preserve">M0 STM32F0 Microcontroller IC 32-Bit </t>
+    <t xml:space="preserve">STM32F091C</t>
   </si>
   <si>
     <t xml:space="preserve">497-18516-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">U2</t>
+    <t xml:space="preserve">U1</t>
   </si>
   <si>
     <t xml:space="preserve">Texas Instruments</t>
@@ -511,21 +473,18 @@
     <t xml:space="preserve">TCAN330GDCNT</t>
   </si>
   <si>
-    <t xml:space="preserve"> Transceiver CANbus SOT-23-8 </t>
+    <t xml:space="preserve">TCAN330</t>
   </si>
   <si>
     <t xml:space="preserve">296-44211-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">U5</t>
+    <t xml:space="preserve">U10</t>
   </si>
   <si>
     <t xml:space="preserve">TPS62111RSA</t>
   </si>
   <si>
-    <t xml:space="preserve">Buck, Regulator, Positive Fixed 3.3V, Output 1.5A, 16-VQFN</t>
-  </si>
-  <si>
     <t xml:space="preserve">296-37681-2-ND</t>
   </si>
   <si>
@@ -535,7 +494,7 @@
     <t xml:space="preserve">1909763-1</t>
   </si>
   <si>
-    <t xml:space="preserve">U.FL (UMCC) Connector Jack, Male Pin 50Ohm</t>
+    <t xml:space="preserve">U.FL</t>
   </si>
   <si>
     <t xml:space="preserve">A118077CT-ND</t>
@@ -551,6 +510,12 @@
   </si>
   <si>
     <t xml:space="preserve">Rev</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.0r0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">new BOM for version 4r0</t>
   </si>
   <si>
     <t xml:space="preserve">3.3r1</t>
@@ -599,16 +564,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="16">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -627,28 +592,131 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Sans"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="0"/>
-      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Sans"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="0"/>
-      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -656,8 +724,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -681,45 +764,177 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="22">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFCC0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF006600"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF996600"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFDDDDDD"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCCCC"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -728,13 +943,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I1048576"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.7"/>
@@ -872,25 +1087,25 @@
       <c r="E8" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="H8" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="I8" s="0" t="s">
         <v>24</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>19</v>
@@ -899,135 +1114,135 @@
         <v>20</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>27</v>
-      </c>
-      <c r="F9" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>34</v>
+      <c r="I10" s="5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="G11" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I11" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I12" s="0" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="G13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="H13" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H13" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I13" s="0" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1035,65 +1250,65 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H15" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I15" s="0" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>19</v>
@@ -1102,135 +1317,135 @@
         <v>20</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G16" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H16" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I16" s="0" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G17" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H17" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I17" s="0" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="G18" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H18" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I18" s="0" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" s="0" t="s">
-        <v>74</v>
+        <v>68</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="G19" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H19" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H19" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I19" s="0" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="F20" s="0" t="s">
-        <v>79</v>
+        <v>73</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="G20" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H20" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I20" s="0" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1238,28 +1453,28 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="F21" s="0" t="s">
-        <v>83</v>
+        <v>78</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="G21" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H21" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H21" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I21" s="0" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1267,28 +1482,28 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" s="0" t="s">
+        <v>83</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G22" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H22" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="0" t="s">
         <v>86</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G22" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I22" s="0" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1296,28 +1511,28 @@
         <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="E23" s="0" t="s">
+        <v>89</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="G23" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H23" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>92</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="G23" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H23" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I23" s="0" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1325,135 +1540,144 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>98</v>
+        <v>94</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="G24" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H24" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H24" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I24" s="0" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G25" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="H25" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="E26" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="0" t="s">
+      <c r="G26" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H26" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I26" s="0" t="s">
         <v>105</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I26" s="0" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="0" t="s">
+      <c r="G27" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H27" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="0" t="s">
+      <c r="I27" s="0" t="s">
         <v>111</v>
-      </c>
-      <c r="G27" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I27" s="0" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="E28" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="E28" s="0" t="s">
+      <c r="G28" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H28" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I28" s="0" t="s">
         <v>115</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="G28" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H28" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I28" s="0" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1461,28 +1685,28 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E29" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="F29" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G29" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H29" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="0" t="s">
         <v>119</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>120</v>
-      </c>
-      <c r="G29" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H29" s="0" t="s">
-        <v>121</v>
-      </c>
-      <c r="I29" s="0" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1490,144 +1714,117 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="E31" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="0" t="s">
-        <v>130</v>
+        <v>124</v>
+      </c>
+      <c r="F31" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H31" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I31" s="0" t="s">
-        <v>131</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="E32" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="F32" s="0" t="s">
-        <v>134</v>
-      </c>
       <c r="G32" s="0" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>137</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>138</v>
-      </c>
-      <c r="F33" s="0" t="s">
-        <v>139</v>
+        <v>131</v>
+      </c>
+      <c r="F33" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="H33" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I33" s="0" t="s">
-        <v>140</v>
+        <v>22</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>141</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="E34" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="F34" s="0" t="s">
-        <v>143</v>
+        <v>17</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1635,77 +1832,77 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="D35" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E35" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>102</v>
+        <v>134</v>
+      </c>
+      <c r="C35" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="G35" s="0" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>146</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>101</v>
+        <v>137</v>
+      </c>
+      <c r="C36" s="7" t="s">
+        <v>19</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>36</v>
+        <v>138</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="F36" s="0" t="s">
-        <v>148</v>
-      </c>
-      <c r="G36" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="G36" s="0" t="s">
+        <v>85</v>
+      </c>
+      <c r="H36" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="H36" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="I36" s="0" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>150</v>
-      </c>
-      <c r="C37" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="C37" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="F37" s="0" t="s">
-        <v>153</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>52</v>
+        <v>144</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="G37" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1713,28 +1910,28 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C38" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="G38" s="5" t="s">
-        <v>52</v>
+        <v>150</v>
+      </c>
+      <c r="G38" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1742,173 +1939,157 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>160</v>
-      </c>
-      <c r="C39" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>52</v>
+        <v>153</v>
+      </c>
+      <c r="G39" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>165</v>
-      </c>
-      <c r="C40" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>19</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>161</v>
+        <v>77</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>166</v>
-      </c>
-      <c r="F40" s="0" t="s">
-        <v>167</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>52</v>
+        <v>156</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G40" s="0" t="s">
+        <v>85</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>169</v>
-      </c>
-      <c r="C41" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E41" s="0" t="s">
-        <v>170</v>
-      </c>
-      <c r="F41" s="0" t="s">
-        <v>171</v>
-      </c>
-      <c r="G41" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H41" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="I41" s="0" t="s">
-        <v>172</v>
-      </c>
+      <c r="C41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>177</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>178</v>
+        <v>163</v>
+      </c>
+      <c r="B45" s="8" t="n">
+        <v>44013</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>179</v>
+        <v>164</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>180</v>
-      </c>
-      <c r="B46" s="0" t="n">
-        <v>43805</v>
+        <v>165</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>166</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
       <c r="B47" s="0" t="n">
-        <v>43681</v>
+        <v>43805</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
       <c r="B48" s="0" t="n">
-        <v>43520</v>
+        <v>43681</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>186</v>
-      </c>
-      <c r="B49" s="0" t="s">
-        <v>187</v>
+        <v>172</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>43520</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>188</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>189</v>
+        <v>174</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+        <v>176</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>178</v>
+      </c>
+    </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -2853,11 +3034,7 @@
     <row r="993" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="994" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="995" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="996" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
updated attributes and BOM
</commit_message>
<xml_diff>
--- a/oresat-proto-card-bom.xlsx
+++ b/oresat-proto-card-bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="188">
   <si>
     <t xml:space="preserve">Bill Of Materials for OreSat Prototype Card</t>
   </si>
@@ -88,6 +88,9 @@
     <t xml:space="preserve">RC0603JR-070RL</t>
   </si>
   <si>
+    <t xml:space="preserve">RES SMD 0 OHM JUMPER 1/10W 0603</t>
+  </si>
+  <si>
     <t xml:space="preserve">Y</t>
   </si>
   <si>
@@ -103,6 +106,9 @@
     <t xml:space="preserve">RC0603FR-0710RL</t>
   </si>
   <si>
+    <t xml:space="preserve">10 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603</t>
+  </si>
+  <si>
     <t xml:space="preserve">311-10.0HRCT-ND</t>
   </si>
   <si>
@@ -112,8 +118,10 @@
     <t xml:space="preserve">RC0603FR-07100RL</t>
   </si>
   <si>
-    <t xml:space="preserve">311-100HRCT-ND
-</t>
+    <t xml:space="preserve">100 Ohms ±1% 0.1W, 1/10W Chip Resistor 0603</t>
+  </si>
+  <si>
+    <t xml:space="preserve">311-100HRCT-ND</t>
   </si>
   <si>
     <t xml:space="preserve">R64</t>
@@ -125,7 +133,7 @@
     <t xml:space="preserve">CSR1206FTR100</t>
   </si>
   <si>
-    <t xml:space="preserve">100m</t>
+    <t xml:space="preserve">100 mOhms ±1% 0.5W, 1/2W Chip Resistor 1206</t>
   </si>
   <si>
     <t xml:space="preserve">CSR1206FTR100CT-ND</t>
@@ -140,7 +148,7 @@
     <t xml:space="preserve">CL05B104KO5NNNC</t>
   </si>
   <si>
-    <t xml:space="preserve">100n</t>
+    <t xml:space="preserve">0.1µF ±10% 16V Ceramic Capacitor X7R 0402</t>
   </si>
   <si>
     <t xml:space="preserve">1276-1001-1-ND</t>
@@ -152,7 +160,7 @@
     <t xml:space="preserve">RNCP0603FTD10K0</t>
   </si>
   <si>
-    <t xml:space="preserve">10k</t>
+    <t xml:space="preserve">10 kOhms ±1% 0.125W, 1/8W Chip Resistor 0603</t>
   </si>
   <si>
     <t xml:space="preserve">RNCP0603FTD10K0CT-ND</t>
@@ -164,7 +172,7 @@
     <t xml:space="preserve">CL21B106KOQNNNG</t>
   </si>
   <si>
-    <t xml:space="preserve">10u</t>
+    <t xml:space="preserve">10µF ±10% 16V Ceramic Capacitor X7R 0805</t>
   </si>
   <si>
     <t xml:space="preserve">1276-6472-1-ND</t>
@@ -179,7 +187,7 @@
     <t xml:space="preserve">ECS-160-10-36Q-ES-TR</t>
   </si>
   <si>
-    <t xml:space="preserve">16MHZ-2.5x2mm</t>
+    <t xml:space="preserve">16MHz ±30ppm Crystal 10pF 80 Ohms</t>
   </si>
   <si>
     <t xml:space="preserve">XC2181CT-ND</t>
@@ -191,7 +199,7 @@
     <t xml:space="preserve">RC0603FR-071ML</t>
   </si>
   <si>
-    <t xml:space="preserve">1M</t>
+    <t xml:space="preserve">1 MOhms ±1% 0.1W, 1/10W Chip Resistor 0603</t>
   </si>
   <si>
     <t xml:space="preserve">311-1.00MHRCT-ND</t>
@@ -203,7 +211,7 @@
     <t xml:space="preserve">CC0603KRX5R7BB105</t>
   </si>
   <si>
-    <t xml:space="preserve">1u</t>
+    <t xml:space="preserve">1µF ±10% 16V Ceramic Capacitor X5R 0603</t>
   </si>
   <si>
     <t xml:space="preserve">311-1444-1-ND</t>
@@ -218,7 +226,7 @@
     <t xml:space="preserve">ERA-3AEB272V</t>
   </si>
   <si>
-    <t xml:space="preserve">2.7k</t>
+    <t xml:space="preserve">2.7 kOhms ±0.1% 0.1W, 1/10W Chip Resistor 0603</t>
   </si>
   <si>
     <t xml:space="preserve">P2.7KDBCT-ND</t>
@@ -230,7 +238,7 @@
     <t xml:space="preserve">CL05C200JB51PNC</t>
   </si>
   <si>
-    <t xml:space="preserve">20p</t>
+    <t xml:space="preserve">20pF ±5% 50V Ceramic Capacitor C0G, NP0 0402</t>
   </si>
   <si>
     <t xml:space="preserve">1276-6601-1-ND</t>
@@ -245,7 +253,7 @@
     <t xml:space="preserve">GRM21BD71A226ME44L</t>
   </si>
   <si>
-    <t xml:space="preserve">22u</t>
+    <t xml:space="preserve">22µF ±20% 10V Ceramic Capacitor X7T 0805</t>
   </si>
   <si>
     <t xml:space="preserve">490-9959-1-ND</t>
@@ -260,7 +268,7 @@
     <t xml:space="preserve">CRGCQ0603F330K</t>
   </si>
   <si>
-    <t xml:space="preserve">330k</t>
+    <t xml:space="preserve">330 kOhms ±1% 0.1W, 1/10W Chip Resistor 0603 </t>
   </si>
   <si>
     <t xml:space="preserve">A129718CT-ND</t>
@@ -275,7 +283,7 @@
     <t xml:space="preserve">ECS-MPI4040R4-6R8-R</t>
   </si>
   <si>
-    <t xml:space="preserve">6.8u</t>
+    <t xml:space="preserve">6.8µH Shielded Inductor 2.4A 91mOhm</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -293,13 +301,13 @@
     <t xml:space="preserve">IN-S63AT5A</t>
   </si>
   <si>
-    <t xml:space="preserve">AMBER</t>
+    <t xml:space="preserve">Amber 605nm LED Indication - Discrete 1.9V 0603 </t>
   </si>
   <si>
     <t xml:space="preserve">1830-1064-1-ND</t>
   </si>
   <si>
-    <t xml:space="preserve">Q10</t>
+    <t xml:space="preserve">Q1</t>
   </si>
   <si>
     <t xml:space="preserve">Diodes Inc</t>
@@ -308,6 +316,9 @@
     <t xml:space="preserve">DMP2240UDM</t>
   </si>
   <si>
+    <t xml:space="preserve">2 P-Channel (Dual) 20V 2A 600mW Surface Mount SOT-26</t>
+  </si>
+  <si>
     <t xml:space="preserve">DMP2240UDMDICT-ND</t>
   </si>
   <si>
@@ -320,7 +331,7 @@
     <t xml:space="preserve">SML-E12M8WT86</t>
   </si>
   <si>
-    <t xml:space="preserve">GREEN</t>
+    <t xml:space="preserve">Green 572nm LED Indication - Discrete 2.2V 0603</t>
   </si>
   <si>
     <t xml:space="preserve">511-1584-1-ND</t>
@@ -335,7 +346,7 @@
     <t xml:space="preserve">73300-0020</t>
   </si>
   <si>
-    <t xml:space="preserve">J-MOLEX-SMPM-73300-003X</t>
+    <t xml:space="preserve">SMPM Connector Plug, Male Pin 50Ohm Board Edge</t>
   </si>
   <si>
     <t xml:space="preserve">WM10772-ND</t>
@@ -350,7 +361,7 @@
     <t xml:space="preserve">TFM-110-01-L-D-RA </t>
   </si>
   <si>
-    <t xml:space="preserve">J-SAMTEC-TFM-110-X1-XXX-D-RA</t>
+    <t xml:space="preserve">Connector Header Through Hole, Right Angle 20 position 0.050"</t>
   </si>
   <si>
     <t xml:space="preserve">Digikey</t>
@@ -365,7 +376,7 @@
     <t xml:space="preserve">TFM-120-01-L-D-RA</t>
   </si>
   <si>
-    <t xml:space="preserve">J-SAMTEC-TFM-120-X1-XXX-D-RA</t>
+    <t xml:space="preserve">Connector Header Through Hole, Right Angle 40 position 0.050"</t>
   </si>
   <si>
     <t xml:space="preserve">SAM10145-ND </t>
@@ -380,6 +391,9 @@
     <t xml:space="preserve">MAX4211FETE</t>
   </si>
   <si>
+    <t xml:space="preserve">Current Monitor Regulator High-Side 16-TQFN</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAX4211FETE+-ND</t>
   </si>
   <si>
@@ -389,6 +403,9 @@
     <t xml:space="preserve">MAX7310ATE</t>
   </si>
   <si>
+    <t xml:space="preserve">I/O Expander 8 I²C, SMBus 400kHz 16-TQFN</t>
+  </si>
+  <si>
     <t xml:space="preserve">MAX7310ATE+-ND</t>
   </si>
   <si>
@@ -401,6 +418,12 @@
     <t xml:space="preserve">MIC842LYC5</t>
   </si>
   <si>
+    <t xml:space="preserve">Comparator with Voltage Reference Push-Pull SC-70-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">576-2927-1-ND</t>
+  </si>
+  <si>
     <t xml:space="preserve">Q2, Q7</t>
   </si>
   <si>
@@ -443,7 +466,7 @@
     <t xml:space="preserve">PMV45EN2R</t>
   </si>
   <si>
-    <t xml:space="preserve">PMV45EN</t>
+    <t xml:space="preserve">N-Channel 30V 4.1A (Ta) 510mW (Ta), 5W (Tc) TO-236AB</t>
   </si>
   <si>
     <t xml:space="preserve">1727-2307-1-ND</t>
@@ -455,13 +478,13 @@
     <t xml:space="preserve">STMicroelectronics</t>
   </si>
   <si>
-    <t xml:space="preserve">STM32F042K6T7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STM32F091C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">497-18516-ND</t>
+    <t xml:space="preserve">STM32F091CCT6TR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ARM® Cortex®-M0 STM32F0 Microcontroller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">497-18749-1-ND</t>
   </si>
   <si>
     <t xml:space="preserve">U1</t>
@@ -473,7 +496,7 @@
     <t xml:space="preserve">TCAN330GDCNT</t>
   </si>
   <si>
-    <t xml:space="preserve">TCAN330</t>
+    <t xml:space="preserve">Transceiver CANbus SOT-23-8</t>
   </si>
   <si>
     <t xml:space="preserve">296-44211-1-ND</t>
@@ -485,6 +508,9 @@
     <t xml:space="preserve">TPS62111RSA</t>
   </si>
   <si>
+    <t xml:space="preserve">Buck Switching Regulator IC Positive Fixed 3.3V</t>
+  </si>
+  <si>
     <t xml:space="preserve">296-37681-2-ND</t>
   </si>
   <si>
@@ -494,7 +520,7 @@
     <t xml:space="preserve">1909763-1</t>
   </si>
   <si>
-    <t xml:space="preserve">U.FL</t>
+    <t xml:space="preserve">U.FL (UMCC) Connector Jack</t>
   </si>
   <si>
     <t xml:space="preserve">A118077CT-ND</t>
@@ -568,12 +594,13 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -592,131 +619,35 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="24"/>
-      <color rgb="FF000000"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF333333"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="10"/>
-      <color rgb="FF808080"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF996600"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFCC0000"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Sans"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Sans"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Sans"/>
+      <sz val="5.1"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FF800000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF000000"/>
-        <bgColor rgb="FF003300"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF808080"/>
-        <bgColor rgb="FF969696"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
-        <bgColor rgb="FFFFCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -724,23 +655,8 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin">
-        <color rgb="FF808080"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF808080"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF808080"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF808080"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="36">
+  <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -764,70 +680,18 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -842,7 +706,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -851,90 +719,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading" xfId="20" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Text" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Note" xfId="24" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Footnote" xfId="25" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Status" xfId="26" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Good" xfId="27" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Neutral" xfId="28" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Bad" xfId="29" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Warning" xfId="30" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Error" xfId="31" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent" xfId="32" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 1" xfId="33" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 2" xfId="34" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Accent 3" xfId="35" builtinId="53" customBuiltin="true"/>
   </cellStyles>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="FF000000"/>
-      <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFCC0000"/>
-      <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF006600"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF996600"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FFC0C0C0"/>
-      <rgbColor rgb="FF808080"/>
-      <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFDDDDDD"/>
-      <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FFFF00FF"/>
-      <rgbColor rgb="FFFFFF00"/>
-      <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008080"/>
-      <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FF00CCFF"/>
-      <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
-      <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
-      <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCCCC"/>
-      <rgbColor rgb="FF3366FF"/>
-      <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF99CC00"/>
-      <rgbColor rgb="FFFFCC00"/>
-      <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
-      <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
-      <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
-      <rgbColor rgb="FF993366"/>
-      <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -945,8 +737,8 @@
   </sheetPr>
   <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I13" activeCellId="0" sqref="I13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7:I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1087,17 +879,17 @@
       <c r="E8" s="0" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="H8" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1105,7 +897,7 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>19</v>
@@ -1114,19 +906,19 @@
         <v>20</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="F9" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1134,7 +926,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>19</v>
@@ -1143,19 +935,19 @@
         <v>20</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>22</v>
+        <v>31</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1163,28 +955,28 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C11" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>22</v>
+        <v>37</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1192,28 +984,28 @@
         <v>6</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C12" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>22</v>
+        <v>42</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1221,28 +1013,28 @@
         <v>11</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C13" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>22</v>
+        <v>46</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>23</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1250,28 +1042,28 @@
         <v>1</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="C14" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1279,28 +1071,28 @@
         <v>1</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="C15" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1308,7 +1100,7 @@
         <v>2</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C16" s="0" t="s">
         <v>19</v>
@@ -1317,19 +1109,19 @@
         <v>20</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1337,7 +1129,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C17" s="0" t="s">
         <v>19</v>
@@ -1346,19 +1138,19 @@
         <v>20</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1366,28 +1158,28 @@
         <v>6</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="C18" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1395,28 +1187,28 @@
         <v>2</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C19" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1424,28 +1216,28 @@
         <v>1</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C20" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1453,28 +1245,28 @@
         <v>2</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C21" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1482,28 +1274,28 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C22" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1511,28 +1303,28 @@
         <v>2</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C23" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1540,28 +1332,28 @@
         <v>1</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C24" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1569,28 +1361,28 @@
         <v>2</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C25" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>97</v>
+        <v>101</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1598,28 +1390,28 @@
         <v>3</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1627,28 +1419,28 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="C27" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1656,28 +1448,28 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="C28" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1685,28 +1477,28 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C29" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1714,28 +1506,28 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C30" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1743,19 +1535,28 @@
         <v>2</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>123</v>
+        <v>129</v>
       </c>
       <c r="C31" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>124</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>125</v>
+        <v>130</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
+      </c>
+      <c r="H31" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1763,28 +1564,28 @@
         <v>2</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C32" s="0" t="s">
         <v>19</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1792,39 +1593,39 @@
         <v>1</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="C34" s="4" t="s">
-        <v>131</v>
+      <c r="B34" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>139</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1832,19 +1633,19 @@
         <v>1</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1852,28 +1653,28 @@
         <v>2</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>19</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>140</v>
+        <v>148</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>141</v>
+        <v>149</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1881,28 +1682,28 @@
         <v>1</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>142</v>
-      </c>
-      <c r="C37" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>144</v>
+        <v>152</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>145</v>
+        <v>153</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1910,28 +1711,28 @@
         <v>1</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>150</v>
+        <v>158</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1939,28 +1740,28 @@
         <v>1</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>152</v>
-      </c>
-      <c r="C39" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1968,126 +1769,126 @@
         <v>3</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>155</v>
-      </c>
-      <c r="C40" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>19</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C41" s="4"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B43" s="0" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B45" s="8" t="n">
         <v>44013</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>43805</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>43681</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>43520</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>